<commit_message>
Implemented statistics module. Layout change. Massive refactoring.
</commit_message>
<xml_diff>
--- a/sample_dictionary.xlsx
+++ b/sample_dictionary.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="19410" windowHeight="7995"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
   <si>
     <t>odbiti</t>
   </si>
@@ -161,12 +161,6 @@
   </si>
   <si>
     <t>trajati</t>
-  </si>
-  <si>
-    <t>angemessen</t>
-  </si>
-  <si>
-    <t>prikladno</t>
   </si>
   <si>
     <t>ausstehen</t>
@@ -646,7 +640,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -659,31 +653,31 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -708,11 +702,11 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -726,13 +720,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -746,7 +740,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
@@ -755,16 +749,16 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
@@ -773,7 +767,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
@@ -801,214 +795,215 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" t="s">
-        <v>50</v>
+      <c r="A16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" t="s">
-        <v>87</v>
+      <c r="A17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
       <c r="C20" s="2" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>36</v>
+      <c r="A23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>90</v>
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>84</v>
-      </c>
-      <c r="B31" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>14</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" t="s">
         <v>3</v>
       </c>
-      <c r="C35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" t="s">
-        <v>47</v>
+      <c r="C36" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" t="s">
-        <v>22</v>
+      <c r="A37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1026,6 +1021,7 @@
       <c r="A39" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
         <v>26</v>
       </c>
@@ -1042,72 +1038,62 @@
       <c r="A41" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B42" t="s">
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>44</v>
+      <c r="A43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>29</v>
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>23</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="A45" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C45" t="s">
-        <v>24</v>
+      <c r="C45" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>68</v>
-      </c>
-      <c r="B46" t="s">
-        <v>2</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:C408">
-    <sortCondition ref="A409"/>
+  <sortState ref="A1:C47">
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>

</xml_diff>